<commit_message>
Update GRE Vocab - 26 Jan 2022.xlsx
</commit_message>
<xml_diff>
--- a/GRE Vocab - 26 Jan 2022.xlsx
+++ b/GRE Vocab - 26 Jan 2022.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidbi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Projects\Stock_Predict\GRE-Words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC0A5D3-D79B-467A-BD52-7C2868F73BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{51C7E4EE-6BCE-4980-86C9-7353D8DA4AB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="GRE 300" sheetId="5" r:id="rId1"/>
@@ -1560,7 +1559,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1645,24 +1644,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1971,22 +1953,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B67267A-B4C4-44C9-BD53-1D7B48DCE3D9}">
-  <dimension ref="A1:D161"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D162"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" customWidth="1"/>
-    <col min="4" max="4" width="51.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="51.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1998,7 +1980,7 @@
       </c>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2010,7 +1992,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2022,7 +2004,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2034,7 +2016,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2046,7 +2028,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2058,7 +2040,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2070,7 +2052,7 @@
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2082,7 +2064,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2094,7 +2076,7 @@
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2106,7 +2088,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2118,7 +2100,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2130,7 +2112,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2142,7 +2124,7 @@
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2154,7 +2136,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2166,7 +2148,7 @@
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2178,7 +2160,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2190,7 +2172,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2202,7 +2184,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2214,7 +2196,7 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2226,7 +2208,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2238,7 +2220,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2250,7 +2232,7 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2262,7 +2244,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2274,7 +2256,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2286,7 +2268,7 @@
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2298,7 +2280,7 @@
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2310,7 +2292,7 @@
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2322,7 +2304,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2334,7 +2316,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2346,7 +2328,7 @@
       </c>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2358,7 +2340,7 @@
       </c>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2370,7 +2352,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2382,7 +2364,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2394,7 +2376,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2406,7 +2388,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2418,7 +2400,7 @@
       </c>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2430,7 +2412,7 @@
       </c>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2442,7 +2424,7 @@
       </c>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2454,7 +2436,7 @@
       </c>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2466,7 +2448,7 @@
       </c>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2478,7 +2460,7 @@
       </c>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2490,7 +2472,7 @@
       </c>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2502,7 +2484,7 @@
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2514,7 +2496,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2526,7 +2508,7 @@
       </c>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2538,7 +2520,7 @@
       </c>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2550,7 +2532,7 @@
       </c>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2562,7 +2544,7 @@
       </c>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2574,7 +2556,7 @@
       </c>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2586,7 +2568,7 @@
       </c>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2598,7 +2580,7 @@
       </c>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2610,7 +2592,7 @@
       </c>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2622,7 +2604,7 @@
       </c>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2634,7 +2616,7 @@
       </c>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2646,7 +2628,7 @@
       </c>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2658,7 +2640,7 @@
       </c>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2670,7 +2652,7 @@
       </c>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2682,7 +2664,7 @@
       </c>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -2694,7 +2676,7 @@
       </c>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -2706,7 +2688,7 @@
       </c>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2718,7 +2700,7 @@
       </c>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2730,7 +2712,7 @@
       </c>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2742,7 +2724,7 @@
       </c>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -2754,7 +2736,7 @@
       </c>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -2766,7 +2748,7 @@
       </c>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -2778,7 +2760,7 @@
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -2790,7 +2772,7 @@
       </c>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -2802,7 +2784,7 @@
       </c>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -2814,7 +2796,7 @@
       </c>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -2826,7 +2808,7 @@
       </c>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -2838,7 +2820,7 @@
       </c>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -2850,7 +2832,7 @@
       </c>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -2862,7 +2844,7 @@
       </c>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -2874,7 +2856,7 @@
       </c>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -2886,7 +2868,7 @@
       </c>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -2898,7 +2880,7 @@
       </c>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -2910,7 +2892,7 @@
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -2922,7 +2904,7 @@
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -2934,7 +2916,7 @@
       </c>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -2946,7 +2928,7 @@
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -2958,7 +2940,7 @@
       </c>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -2970,7 +2952,7 @@
       </c>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -2982,7 +2964,7 @@
       </c>
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -2994,7 +2976,7 @@
       </c>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -3006,7 +2988,7 @@
       </c>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -3018,7 +3000,7 @@
       </c>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -3030,7 +3012,7 @@
       </c>
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -3042,7 +3024,7 @@
       </c>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -3054,7 +3036,7 @@
       </c>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -3066,7 +3048,7 @@
       </c>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -3080,7 +3062,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -3092,7 +3074,7 @@
       </c>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -3104,7 +3086,7 @@
       </c>
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -3116,7 +3098,7 @@
       </c>
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -3128,7 +3110,7 @@
       </c>
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -3140,7 +3122,7 @@
       </c>
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -3152,7 +3134,7 @@
       </c>
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -3164,7 +3146,7 @@
       </c>
       <c r="D98" s="2"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -3176,7 +3158,7 @@
       </c>
       <c r="D99" s="2"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -3188,7 +3170,7 @@
       </c>
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -3200,7 +3182,7 @@
       </c>
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -3212,7 +3194,7 @@
       </c>
       <c r="D102" s="2"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -3224,7 +3206,7 @@
       </c>
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -3236,7 +3218,7 @@
       </c>
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -3248,7 +3230,7 @@
       </c>
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -3262,7 +3244,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -3274,7 +3256,7 @@
       </c>
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -3286,7 +3268,7 @@
       </c>
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -3298,7 +3280,7 @@
       </c>
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -3312,7 +3294,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -3324,7 +3306,7 @@
       </c>
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -3336,7 +3318,7 @@
       </c>
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -3348,7 +3330,7 @@
       </c>
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -3362,7 +3344,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -3374,7 +3356,7 @@
       </c>
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -3386,7 +3368,7 @@
       </c>
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -3398,7 +3380,7 @@
       </c>
       <c r="D117" s="2"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -3412,7 +3394,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -3424,7 +3406,7 @@
       </c>
       <c r="D119" s="2"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -3436,7 +3418,7 @@
       </c>
       <c r="D120" s="2"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -3450,7 +3432,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -3462,7 +3444,7 @@
       </c>
       <c r="D122" s="6"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -3474,7 +3456,7 @@
       </c>
       <c r="D123" s="6"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -3486,7 +3468,7 @@
       </c>
       <c r="D124" s="6"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -3498,7 +3480,7 @@
       </c>
       <c r="D125" s="6"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -3510,7 +3492,7 @@
       </c>
       <c r="D126" s="6"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -3522,7 +3504,7 @@
       </c>
       <c r="D127" s="6"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -3534,7 +3516,7 @@
       </c>
       <c r="D128" s="6"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -3546,7 +3528,7 @@
       </c>
       <c r="D129" s="6"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -3558,7 +3540,7 @@
       </c>
       <c r="D130" s="6"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -3570,7 +3552,7 @@
       </c>
       <c r="D131" s="6"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -3582,7 +3564,7 @@
       </c>
       <c r="D132" s="6"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -3594,7 +3576,7 @@
       </c>
       <c r="D133" s="6"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -3606,7 +3588,7 @@
       </c>
       <c r="D134" s="6"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="2">
         <v>134</v>
       </c>
@@ -3618,7 +3600,7 @@
       </c>
       <c r="D135" s="6"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
         <v>135</v>
       </c>
@@ -3630,7 +3612,7 @@
       </c>
       <c r="D136" s="6"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
         <v>136</v>
       </c>
@@ -3642,7 +3624,7 @@
       </c>
       <c r="D137" s="6"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>137</v>
       </c>
@@ -3654,7 +3636,7 @@
       </c>
       <c r="D138" s="6"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
         <v>138</v>
       </c>
@@ -3666,7 +3648,7 @@
       </c>
       <c r="D139" s="6"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="2">
         <v>139</v>
       </c>
@@ -3678,7 +3660,7 @@
       </c>
       <c r="D140" s="6"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
         <v>140</v>
       </c>
@@ -3690,7 +3672,7 @@
       </c>
       <c r="D141" s="6"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="2">
         <v>141</v>
       </c>
@@ -3702,7 +3684,7 @@
       </c>
       <c r="D142" s="6"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
         <v>142</v>
       </c>
@@ -3714,7 +3696,7 @@
       </c>
       <c r="D143" s="6"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
         <v>143</v>
       </c>
@@ -3726,7 +3708,7 @@
       </c>
       <c r="D144" s="6"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -3738,7 +3720,7 @@
       </c>
       <c r="D145" s="6"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
         <v>145</v>
       </c>
@@ -3750,7 +3732,7 @@
       </c>
       <c r="D146" s="6"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="2">
         <v>146</v>
       </c>
@@ -3762,7 +3744,7 @@
       </c>
       <c r="D147" s="6"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
         <v>147</v>
       </c>
@@ -3774,7 +3756,7 @@
       </c>
       <c r="D148" s="6"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -3786,7 +3768,7 @@
       </c>
       <c r="D149" s="6"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="2">
         <v>149</v>
       </c>
@@ -3800,7 +3782,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -3812,7 +3794,7 @@
       </c>
       <c r="D151" s="6"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
         <v>151</v>
       </c>
@@ -3824,7 +3806,7 @@
       </c>
       <c r="D152" s="6"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -3836,7 +3818,7 @@
       </c>
       <c r="D153" s="6"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -3848,7 +3830,7 @@
       </c>
       <c r="D154" s="6"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="2">
         <v>154</v>
       </c>
@@ -3860,7 +3842,7 @@
       </c>
       <c r="D155" s="6"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="2">
         <v>155</v>
       </c>
@@ -3872,7 +3854,7 @@
       </c>
       <c r="D156" s="6"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="2">
         <v>156</v>
       </c>
@@ -3884,7 +3866,7 @@
       </c>
       <c r="D157" s="6"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="2">
         <v>157</v>
       </c>
@@ -3896,7 +3878,7 @@
       </c>
       <c r="D158" s="6"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="2">
         <v>158</v>
       </c>
@@ -3908,7 +3890,7 @@
       </c>
       <c r="D159" s="6"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
         <v>159</v>
       </c>
@@ -3920,7 +3902,7 @@
       </c>
       <c r="D160" s="6"/>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="2">
         <v>160</v>
       </c>
@@ -3931,6 +3913,11 @@
         <v>346</v>
       </c>
       <c r="D161" s="6"/>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162" s="2">
+        <v>160</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3939,7 +3926,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664DE637-B043-4B46-A6B0-3F58A12984AE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
@@ -3947,14 +3934,14 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -3965,7 +3952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>69</v>
       </c>
@@ -3973,7 +3960,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>71</v>
       </c>
@@ -3981,7 +3968,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>81</v>
       </c>
@@ -3989,7 +3976,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>84</v>
       </c>
@@ -3997,7 +3984,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>86</v>
       </c>
@@ -4005,7 +3992,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>94</v>
       </c>
@@ -4019,20 +4006,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6DC6FA-DC0B-47A6-8D17-DEB101FE8219}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="42.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="42.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -4043,7 +4030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>179</v>
       </c>
@@ -4051,7 +4038,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>185</v>
       </c>
@@ -4065,19 +4052,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F3CACA-3E97-429B-B7A7-409750E80E86}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="78.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="78.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -4088,7 +4075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>357</v>
       </c>
@@ -4096,7 +4083,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>359</v>
       </c>
@@ -4104,7 +4091,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>361</v>
       </c>
@@ -4112,7 +4099,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>363</v>
       </c>
@@ -4120,7 +4107,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>365</v>
       </c>
@@ -4128,7 +4115,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>367</v>
       </c>
@@ -4136,7 +4123,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>370</v>
       </c>
@@ -4144,7 +4131,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>372</v>
       </c>
@@ -4152,7 +4139,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>374</v>
       </c>
@@ -4166,20 +4153,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8BE501-0A60-4C46-B977-290D1D72852D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C7"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="107.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="107.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>181</v>
       </c>
@@ -4187,7 +4174,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>183</v>
       </c>
@@ -4195,7 +4182,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>368</v>
       </c>
@@ -4203,7 +4190,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>187</v>
       </c>
@@ -4211,7 +4198,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>246</v>
       </c>
@@ -4219,7 +4206,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>295</v>
       </c>
@@ -4227,7 +4214,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>355</v>
       </c>
@@ -4242,20 +4229,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7C3A9F-5AF6-4B97-9327-95042A785AC5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="82.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="82.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>

</xml_diff>